<commit_message>
EPBDS-7689 Access to Condition parameters in another Condition expression Rules and Smart Rules (external conditions). Any order is supported.
--HG--
branch : EPBDS-7689
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7689_ConditionParameters.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7689_ConditionParameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\Tutorial 1 - Introduction to Decision Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-7689_ConditionParameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BC8456-A653-4F47-949C-C19C069F3EC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E364CC57-51AF-437F-96F8-8AF2F13F08C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="2745" windowWidth="21600" windowHeight="12855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,12 +349,99 @@
         </r>
       </text>
     </comment>
+    <comment ref="G68" authorId="0" shapeId="0" xr:uid="{5B330431-54A9-4D32-9475-26331A5FC58A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>The condition equals to driverAge == 
+ageType</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C69" authorId="0" shapeId="0" xr:uid="{B646961A-B858-4AAC-92C9-300DDFA21D8D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>The condition equals to driverAge == 
+ageType</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G69" authorId="0" shapeId="0" xr:uid="{CE2FA4E8-455A-4D96-A3AE-C3CCC904CACF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>The definition equals to, for example, String ageType</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C70" authorId="0" shapeId="0" xr:uid="{253654C1-6404-4FC7-9963-50501B972050}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>The definition equals to, for example, String ageType</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C86" authorId="0" shapeId="0" xr:uid="{5CAC007D-1394-4960-93D3-0C34000E21B0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>The condition equals to driverAge == 
+ageType</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C87" authorId="0" shapeId="0" xr:uid="{80B380A5-8D95-43ED-8D69-93EE4ACF6600}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>The definition equals to, for example, String ageType</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="51">
   <si>
     <t>C1</t>
   </si>
@@ -587,6 +674,108 @@
   </si>
   <si>
     <t>$C1.$C1.equals("Young Driver") ? ret : 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">driverAge </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules Double </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Table4</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (String driverAge, String driverMaritalStatus)</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Table4 Table4Test</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules Double </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Table5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (String driverAge, String driverMaritalStatus)</t>
+    </r>
+  </si>
+  <si>
+    <t>$C1.x2 == x2 &amp;&amp; x5 == "A1" || $A1.x4 == "A1"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rules Double </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Table6</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (String driverAge, String driverMaritalStatus)</t>
+    </r>
+  </si>
+  <si>
+    <t>x5 == 0</t>
+  </si>
+  <si>
+    <t>Test Table6 Table6Test</t>
+  </si>
+  <si>
+    <t>x5 == "0"</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Double x5</t>
   </si>
 </sst>
 </file>
@@ -1066,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C0DC64-11BA-4F10-8EC3-B7EB2A03B20A}">
-  <dimension ref="A2:O61"/>
+  <dimension ref="A2:O106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1134,7 +1323,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -1742,6 +1931,286 @@
         <v>500</v>
       </c>
     </row>
+    <row r="67" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B67" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="G67" s="8"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B68" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G68" s="8"/>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B69" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="8"/>
+      <c r="G69" s="8"/>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B70" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G70" s="8"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B71" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G71" s="8"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B72" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B75" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B76" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B77" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B78" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B84" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B85" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B86" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B87" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E87" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B88" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E88" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B89" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="8">
+        <v>0</v>
+      </c>
+      <c r="E89" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B94" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B95" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B96" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="8"/>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B97" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D97" s="8"/>
+      <c r="E97" s="8"/>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B98" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" s="8"/>
+      <c r="E98" s="8"/>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B99" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="8">
+        <v>0</v>
+      </c>
+      <c r="D99" s="8"/>
+      <c r="E99" s="8"/>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B103" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C103" s="8"/>
+      <c r="D103" s="8"/>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B104" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B105" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D105" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B106" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C106" s="8"/>
+      <c r="D106" s="8">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>